<commit_message>
Update credibility explanation and Belgium data
</commit_message>
<xml_diff>
--- a/data/traffic_light_indicators_data-2021-06-04.xlsx
+++ b/data/traffic_light_indicators_data-2021-06-04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Almut B\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maarten/Documents/clients/stefanscheuer/buildings-dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF8D88F-D66A-4A81-A878-D1344AAB4FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F533B5C-D58F-9649-88A5-BF790565DE1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C3AFBA72-B1BC-4A11-A93A-E672CAD481DA}"/>
+    <workbookView xWindow="-100" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{C3AFBA72-B1BC-4A11-A93A-E672CAD481DA}"/>
   </bookViews>
   <sheets>
     <sheet name="ban_gas_grid" sheetId="1" r:id="rId1"/>
@@ -246,7 +246,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -262,7 +262,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -564,17 +564,17 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -588,7 +588,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -602,7 +602,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -610,7 +610,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -618,7 +618,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -632,7 +632,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -643,7 +643,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -651,7 +651,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -659,7 +659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -681,7 +681,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -689,7 +689,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -700,7 +700,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -708,7 +708,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -716,7 +716,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -724,7 +724,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -732,7 +732,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -743,7 +743,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -751,7 +751,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -759,7 +759,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -773,7 +773,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -787,7 +787,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -795,7 +795,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -803,7 +803,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -811,7 +811,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -819,7 +819,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -827,7 +827,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -835,7 +835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -853,16 +853,16 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -879,15 +879,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -895,7 +895,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -903,7 +903,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -911,7 +911,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -919,7 +919,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -927,7 +927,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -935,7 +935,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -943,7 +943,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -951,7 +951,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -959,7 +959,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -967,7 +967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -975,7 +975,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -983,7 +983,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -991,7 +991,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -999,7 +999,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
     </row>
   </sheetData>

</xml_diff>